<commit_message>
Sửa lỗi api báo cáo
</commit_message>
<xml_diff>
--- a/EVN.Api/Templates/BaoCaoChiTietGiamSatTienDo.xlsx
+++ b/EVN.Api/Templates/BaoCaoChiTietGiamSatTienDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeEvn\GiamSatTrungAp\GiamSatTrungAp_BE\EVN.Api\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EVN\UngDungTrungAp\EVN.Api\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414A489A-4417-4A75-B779-B2454C9098D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E54395D-0F98-4DFC-AE2E-0C1628B9DA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85D203D3-93C0-4CC7-9E1A-8B7A758889F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85D203D3-93C0-4CC7-9E1A-8B7A758889F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,17 +144,23 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -188,6 +194,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -195,42 +214,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -241,14 +248,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -622,92 +647,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DBECFB-CE9C-4F4A-B3F6-405E283682E3}">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="20" width="11" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="18.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="3" customWidth="1"/>
+    <col min="7" max="8" width="11" style="3" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="55.88671875" style="3" customWidth="1"/>
+    <col min="11" max="20" width="11" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-    </row>
-    <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+    </row>
+    <row r="2" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-    </row>
-    <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -745,223 +776,1044 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="Q6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="S6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="T6" s="10" t="s">
+      <c r="T6" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="3"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="6"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+    </row>
+    <row r="9" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+    </row>
+    <row r="11" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="4"/>
+    </row>
+    <row r="12" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+    </row>
+    <row r="13" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+    </row>
+    <row r="14" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+    </row>
+    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+    </row>
+    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+    </row>
+    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+    </row>
+    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+    </row>
+    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+    </row>
+    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+    </row>
+    <row r="25" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+    </row>
+    <row r="26" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+    </row>
+    <row r="27" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+    </row>
+    <row r="28" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+    </row>
+    <row r="29" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+    </row>
+    <row r="30" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+    </row>
+    <row r="31" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+    </row>
+    <row r="32" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+    </row>
+    <row r="33" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+    </row>
+    <row r="34" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+    </row>
+    <row r="35" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+    </row>
+    <row r="36" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+    </row>
+    <row r="37" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+    </row>
+    <row r="38" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+    </row>
+    <row r="39" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+    </row>
+    <row r="40" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+    </row>
+    <row r="41" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+    </row>
+    <row r="42" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
+    </row>
+    <row r="43" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+    </row>
+    <row r="44" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="7"/>
+    </row>
+    <row r="45" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
+    </row>
+    <row r="46" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
+    </row>
+    <row r="47" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
+    </row>
+    <row r="48" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="7"/>
+    </row>
+    <row r="49" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="7"/>
+    </row>
+    <row r="50" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="Q6:Q8"/>
+    <mergeCell ref="R6:R8"/>
+    <mergeCell ref="S6:S8"/>
     <mergeCell ref="M6:M8"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="A2:T2"/>
@@ -978,13 +1830,6 @@
     <mergeCell ref="J6:J8"/>
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="L6:L8"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="P6:P8"/>
-    <mergeCell ref="Q6:Q8"/>
-    <mergeCell ref="R6:R8"/>
-    <mergeCell ref="S6:S8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>